<commit_message>
PROVA - risolto problema LS1
</commit_message>
<xml_diff>
--- a/PS-VRP/Dati_output/Problemi_schedulazione_commesse.xlsx
+++ b/PS-VRP/Dati_output/Problemi_schedulazione_commesse.xlsx
@@ -452,7 +452,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,12 +484,23 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>253668</v>
+        <v>253393</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>45910.58333333334</v>
+        <v>45912.58333333334</v>
       </c>
       <c r="C2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>253392</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>45911.58333333334</v>
+      </c>
+      <c r="C3" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
PROVA - spostate commesse esterne non tassative al gruppo 2
</commit_message>
<xml_diff>
--- a/PS-VRP/Dati_output/Problemi_schedulazione_commesse.xlsx
+++ b/PS-VRP/Dati_output/Problemi_schedulazione_commesse.xlsx
@@ -452,7 +452,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,10 +484,10 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>253393</v>
+        <v>253371</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>45912.58333333334</v>
+        <v>45910.58333333334</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -495,12 +495,124 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>253392</v>
+        <v>253367</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>45911.58333333334</v>
       </c>
       <c r="C3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>253472</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>45912.58333333334</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>253549</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>45912.58333333334</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>253392</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>45911.58333333334</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>253393</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>45912.58333333334</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>253295</v>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>45911.58333333334</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>252397</v>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>45911.58333333334</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>253244</v>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>45912.58333333334</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>252274</v>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>45911.58333333334</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>253668</v>
+      </c>
+      <c r="B12" s="1" t="n">
+        <v>45910.58333333334</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>252741</v>
+      </c>
+      <c r="B13" s="1" t="n">
+        <v>45911.58333333334</v>
+      </c>
+      <c r="C13" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
PROVA - re-introdotta differenza minuti vs ore nel calcolo del delta per le LS; alcuni cambi QOL
</commit_message>
<xml_diff>
--- a/PS-VRP/Dati_output/Problemi_schedulazione_commesse.xlsx
+++ b/PS-VRP/Dati_output/Problemi_schedulazione_commesse.xlsx
@@ -452,7 +452,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,7 +484,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>253371</v>
+        <v>253522</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>45910.58333333334</v>
@@ -495,10 +495,10 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>253367</v>
+        <v>253472</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>45911.58333333334</v>
+        <v>45912.58333333334</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
@@ -506,10 +506,10 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>253472</v>
+        <v>253392</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>45912.58333333334</v>
+        <v>45911.58333333334</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
@@ -517,7 +517,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>253549</v>
+        <v>253393</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>45912.58333333334</v>
@@ -528,10 +528,10 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>253392</v>
+        <v>253376</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>45911.58333333334</v>
+        <v>45910.58333333334</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
@@ -539,31 +539,31 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>253393</v>
+        <v>253295</v>
       </c>
       <c r="B7" s="1" t="n">
-        <v>45912.58333333334</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>253295</v>
-      </c>
-      <c r="B8" s="1" t="n">
         <v>45911.58333333334</v>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>252529</v>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>45910.58333333334</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+    </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>252397</v>
+        <v>252274</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>45911.58333333334</v>
@@ -585,7 +585,7 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>252274</v>
+        <v>252397</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>45911.58333333334</v>
@@ -596,10 +596,10 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>253668</v>
+        <v>253549</v>
       </c>
       <c r="B12" s="1" t="n">
-        <v>45910.58333333334</v>
+        <v>45912.58333333334</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
@@ -607,12 +607,56 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
+        <v>253261</v>
+      </c>
+      <c r="B13" s="1" t="n">
+        <v>45910.58333333334</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>244743</v>
+      </c>
+      <c r="B14" s="1" t="n">
+        <v>45910.58333333334</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>253436</v>
+      </c>
+      <c r="B15" s="1" t="n">
+        <v>45910.58333333334</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
         <v>252741</v>
       </c>
-      <c r="B13" s="1" t="n">
+      <c r="B16" s="1" t="n">
         <v>45911.58333333334</v>
       </c>
-      <c r="C13" t="n">
+      <c r="C16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>253668</v>
+      </c>
+      <c r="B17" s="1" t="n">
+        <v>45910.58333333334</v>
+      </c>
+      <c r="C17" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
PROVA - versione finale;
</commit_message>
<xml_diff>
--- a/PS-VRP/Dati_output/Problemi_schedulazione_commesse.xlsx
+++ b/PS-VRP/Dati_output/Problemi_schedulazione_commesse.xlsx
@@ -452,7 +452,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,10 +484,10 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>254187</v>
+        <v>253974</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>45975.58333333334</v>
+        <v>45980.58333333334</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -495,12 +495,34 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
+        <v>254187</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>45975.58333333334</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>254547</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>45980.58333333334</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
         <v>254967</v>
       </c>
-      <c r="B3" s="1" t="n">
+      <c r="B5" s="1" t="n">
         <v>45981.58333333334</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C5" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
PROVA - scorporato gli aggiornamenti per il ritardo delle varie ricerche locali da return_schedulazione
</commit_message>
<xml_diff>
--- a/PS-VRP/Dati_output/Problemi_schedulazione_commesse.xlsx
+++ b/PS-VRP/Dati_output/Problemi_schedulazione_commesse.xlsx
@@ -452,7 +452,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,10 +484,10 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>253974</v>
+        <v>254187</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>45980.58333333334</v>
+        <v>45975.58333333334</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -495,34 +495,12 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>254187</v>
+        <v>254967</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>45975.58333333334</v>
+        <v>45981.58333333334</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>254547</v>
-      </c>
-      <c r="B4" s="1" t="n">
-        <v>45980.58333333334</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>254967</v>
-      </c>
-      <c r="B5" s="1" t="n">
-        <v>45981.58333333334</v>
-      </c>
-      <c r="C5" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>